<commit_message>
Add Fix and Partial Group Access Modules
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Group_Access_Module.xlsx
+++ b/_DOCUMENTS_/Group_Access_Module.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_PROJECT_\RoyalPetz\_DOCUMENTS_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RoyalPetz\_DOCUMENTS_\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>MAINMENU_manajemenSistem</t>
   </si>
@@ -364,6 +364,78 @@
   </si>
   <si>
     <t>MENU_PENGATURAN_NOMOR_RAK</t>
+  </si>
+  <si>
+    <t>KATEGORI PRODUK</t>
+  </si>
+  <si>
+    <t>SATUAN PRODUK</t>
+  </si>
+  <si>
+    <t>MENU_KATEGORI</t>
+  </si>
+  <si>
+    <t>MENU_SATUAN</t>
+  </si>
+  <si>
+    <t>STOK OPNAME</t>
+  </si>
+  <si>
+    <t>PENYESUAIAN STOK</t>
+  </si>
+  <si>
+    <t>PENERIMAAN BARANG</t>
+  </si>
+  <si>
+    <t>TAMBAH / UPDATE SATUAN</t>
+  </si>
+  <si>
+    <t>MENU_TAMBAH_SATUAN</t>
+  </si>
+  <si>
+    <t>PENGATURAN KONVERSI SATUAN</t>
+  </si>
+  <si>
+    <t>CEK PERMINTAAN BARANG</t>
+  </si>
+  <si>
+    <t>MENU_PENGATURAN_KONVERSI</t>
+  </si>
+  <si>
+    <t>MENU_STOK_OPNAME</t>
+  </si>
+  <si>
+    <t>MENU_PENYESUAIAN_STOK</t>
+  </si>
+  <si>
+    <t>MUTASI_BARANG</t>
+  </si>
+  <si>
+    <t>MENU_MUTASI_BARANG</t>
+  </si>
+  <si>
+    <t>TAMBAH / UPDATE MUTASI BARANG</t>
+  </si>
+  <si>
+    <t>MENU_TAMBAH_MUTASI_BARANG</t>
+  </si>
+  <si>
+    <t>MENU_CEK_PERMINTAAN_BARANG</t>
+  </si>
+  <si>
+    <t>MENU_PENERIMAAN_BARANG</t>
+  </si>
+  <si>
+    <t>PENERIMAAN BARANG DARI MUTASI</t>
+  </si>
+  <si>
+    <t>MENU_PENERIMAAN_BARANG_DARI_MUTASI</t>
+  </si>
+  <si>
+    <t>PENERIMAAN BARANG DARI PO</t>
+  </si>
+  <si>
+    <t>MENU_PENERIMAAN_BARANG_DARI_PO</t>
   </si>
 </sst>
 </file>
@@ -478,16 +550,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -510,21 +579,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,16 +890,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="59.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -830,16 +910,16 @@
       </c>
     </row>
     <row r="2" spans="3:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="8" t="s">
         <v>87</v>
       </c>
     </row>
@@ -847,13 +927,13 @@
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="18">
         <v>1</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="22" t="s">
         <v>88</v>
       </c>
     </row>
@@ -861,29 +941,29 @@
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="21"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="18">
         <v>1</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="22" t="s">
         <v>89</v>
       </c>
     </row>
@@ -891,29 +971,29 @@
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="18"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="18">
         <v>7</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="22" t="s">
         <v>90</v>
       </c>
     </row>
@@ -921,37 +1001,37 @@
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="24"/>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="18"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="18">
         <v>7</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -959,21 +1039,21 @@
       <c r="C14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>1</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="5" t="s">
         <v>92</v>
       </c>
     </row>
@@ -981,13 +1061,13 @@
       <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>1</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -995,13 +1075,13 @@
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>1</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="5" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1009,21 +1089,21 @@
       <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="21"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>1</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="5" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1031,13 +1111,13 @@
       <c r="C20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>1</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="5" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1045,13 +1125,13 @@
       <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21" s="10">
         <v>7</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1059,13 +1139,13 @@
       <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="10">
         <v>3</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1073,13 +1153,13 @@
       <c r="C23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="10">
         <v>3</v>
       </c>
-      <c r="F23" s="16" t="s">
+      <c r="F23" s="5" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1087,13 +1167,13 @@
       <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="10">
         <v>3</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1101,13 +1181,13 @@
       <c r="C25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="10">
         <v>3</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1115,407 +1195,480 @@
       <c r="C26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26" s="10">
         <v>3</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="16"/>
-    </row>
-    <row r="28" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D27" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="18">
+        <v>7</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="16"/>
+      <c r="D29" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="30" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="16"/>
+      <c r="D30" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="10">
+        <v>3</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="31" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="16"/>
-    </row>
-    <row r="32" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D31" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="10">
+        <v>3</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="18">
+        <v>1</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D33" s="16"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="23"/>
     </row>
     <row r="35" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="16"/>
+      <c r="D35" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="36" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="16"/>
+      <c r="D36" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="37" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="16"/>
+      <c r="D37" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="10">
+        <v>7</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="38" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C38" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="16"/>
+      <c r="D38" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="39" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="16"/>
+      <c r="D39" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="10">
+        <v>1</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="40" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="16"/>
+      <c r="D40" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" s="10">
+        <v>7</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="41" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="16"/>
+      <c r="D41" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="10">
+        <v>7</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="42" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="16"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="5"/>
     </row>
     <row r="43" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="16"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="16"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C45" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="16"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C46" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="16"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="5"/>
     </row>
     <row r="47" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="16"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C48" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="16"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="5"/>
     </row>
     <row r="49" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C49" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="16"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C50" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="16"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C51" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="16"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C52" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="16"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C53" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="16"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="5"/>
     </row>
     <row r="54" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C54" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="16"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C55" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="16"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="5"/>
     </row>
     <row r="56" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C56" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="16"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C57" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="16"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C58" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="16"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="59" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C59" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="16"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="5"/>
     </row>
     <row r="60" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C60" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="16"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="5"/>
     </row>
     <row r="61" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C61" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="16"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C62" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="16"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="5"/>
     </row>
     <row r="63" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C63" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="16"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="5"/>
     </row>
     <row r="64" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C64" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="16"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C65" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="16"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C66" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="16"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="67" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="16"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C68" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="16"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C69" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="16"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C70" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="16"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C71" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="16"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="5"/>
     </row>
     <row r="72" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C72" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D72" s="6"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="16"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="5"/>
     </row>
     <row r="73" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C73" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="16"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C74" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="16"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
+  <mergeCells count="18">
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="F32:F34"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D9:D12"/>
@@ -1523,6 +1676,11 @@
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="E9:E12"/>
     <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>